<commit_message>
Edited to fix cost on SOLAR2 as well
</commit_message>
<xml_diff>
--- a/case_input_test_191017.xlsx
+++ b/case_input_test_191017.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinerinaldi/SEMProject/my_new_MEM/SEM-1.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAFF492E-BDC5-8C4B-B9BE-1E35A1AA5DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB735918-EBDA-2C43-A6D3-9F965C3E44C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22620" windowHeight="10960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="B86" s="26">
         <f>N86</f>
-        <v>1.9528741509529837E-2</v>
+        <v>2.1863827843931212E-2</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>93</v>
@@ -4269,8 +4269,8 @@
         <v>94</v>
       </c>
       <c r="E86" s="4"/>
-      <c r="F86" s="8">
-        <v>1851</v>
+      <c r="F86" s="60">
+        <v>2105</v>
       </c>
       <c r="G86" s="61" t="str">
         <f>HYPERLINK("https://www.eia.gov/outlooks/archive/aeo18/assumptions/pdf/electricity.pdf","EIA, AEO2018, Electricity Market Module, Table 2")</f>
@@ -4296,11 +4296,11 @@
       </c>
       <c r="M86" s="28">
         <f>F86*J86+K86</f>
-        <v>171.18543289906683</v>
+        <v>191.65437939088909</v>
       </c>
       <c r="N86" s="29">
         <f>M86/HOURS_PER_YEAR</f>
-        <v>1.9528741509529837E-2</v>
+        <v>2.1863827843931212E-2</v>
       </c>
       <c r="O86" s="8"/>
       <c r="P86" s="8"/>

</xml_diff>